<commit_message>
add names to protocols
</commit_message>
<xml_diff>
--- a/bio_diversity/static/report_templates/stock_code_report_template.xlsx
+++ b/bio_diversity/static/report_templates/stock_code_report_template.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Collection</t>
   </si>
@@ -31,6 +31,9 @@
   </si>
   <si>
     <t>Container</t>
+  </si>
+  <si>
+    <t>Fish In Group</t>
   </si>
 </sst>
 </file>
@@ -518,12 +521,13 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -872,7 +876,7 @@
   <dimension ref="A1:U2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -880,6 +884,8 @@
     <col min="1" max="1" width="12.28515625" customWidth="1"/>
     <col min="2" max="2" width="17" customWidth="1"/>
     <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" customWidth="1"/>
+    <col min="5" max="5" width="13.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.25">
@@ -904,18 +910,21 @@
       <c r="T1" s="2"/>
       <c r="U1" s="2"/>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="2" t="s">
         <v>3</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add to stock code report
</commit_message>
<xml_diff>
--- a/bio_diversity/static/report_templates/stock_code_report_template.xlsx
+++ b/bio_diversity/static/report_templates/stock_code_report_template.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Collection</t>
   </si>
@@ -35,6 +35,15 @@
   <si>
     <t>Fish In Group</t>
   </si>
+  <si>
+    <t>Details</t>
+  </si>
+  <si>
+    <t>Gender</t>
+  </si>
+  <si>
+    <t>Still Valid</t>
+  </si>
 </sst>
 </file>
 
@@ -180,7 +189,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -360,8 +369,14 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -473,6 +488,15 @@
       </top>
       <bottom style="double">
         <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -521,13 +545,14 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -876,7 +901,7 @@
   <dimension ref="A1:U2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -910,21 +935,30 @@
       <c r="T1" s="2"/>
       <c r="U1" s="2"/>
     </row>
-    <row r="2" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:21" s="5" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="6" t="s">
         <v>4</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add group column to stock code report
</commit_message>
<xml_diff>
--- a/bio_diversity/static/report_templates/stock_code_report_template.xlsx
+++ b/bio_diversity/static/report_templates/stock_code_report_template.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Collection</t>
   </si>
@@ -43,6 +43,9 @@
   </si>
   <si>
     <t>Still Valid</t>
+  </si>
+  <si>
+    <t>Group</t>
   </si>
 </sst>
 </file>
@@ -898,10 +901,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U2"/>
+  <dimension ref="A1:V2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -909,19 +912,21 @@
     <col min="1" max="1" width="12.28515625" customWidth="1"/>
     <col min="2" max="2" width="17" customWidth="1"/>
     <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.28515625" customWidth="1"/>
-    <col min="5" max="5" width="13.85546875" customWidth="1"/>
-    <col min="8" max="8" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.85546875" customWidth="1"/>
+    <col min="5" max="5" width="11.28515625" customWidth="1"/>
+    <col min="6" max="6" width="13.85546875" customWidth="1"/>
+    <col min="8" max="8" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B1" s="2"/>
       <c r="C1" s="1"/>
-      <c r="D1" s="2"/>
+      <c r="D1" s="1"/>
       <c r="E1" s="2"/>
-      <c r="F1" s="3"/>
+      <c r="F1" s="2"/>
       <c r="G1" s="3"/>
-      <c r="H1" s="2"/>
+      <c r="H1" s="3"/>
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
       <c r="K1" s="2"/>
@@ -929,14 +934,15 @@
       <c r="M1" s="2"/>
       <c r="N1" s="2"/>
       <c r="O1" s="2"/>
-      <c r="P1" s="4"/>
-      <c r="Q1" s="2"/>
+      <c r="P1" s="2"/>
+      <c r="Q1" s="4"/>
       <c r="R1" s="2"/>
       <c r="S1" s="2"/>
       <c r="T1" s="2"/>
       <c r="U1" s="2"/>
+      <c r="V1" s="2"/>
     </row>
-    <row r="2" spans="1:21" s="5" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:22" s="5" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>1</v>
       </c>
@@ -947,18 +953,21 @@
         <v>0</v>
       </c>
       <c r="D2" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="F2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="G2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="H2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="I2" s="6" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>